<commit_message>
add one DP question
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -50,6 +50,21 @@
   </si>
   <si>
     <t>Array</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Count number of binary strings without consecutive 1’s</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Boolean Parenthesization Problem</t>
+  </si>
+  <si>
+    <t>medium</t>
   </si>
 </sst>
 </file>
@@ -394,22 +409,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -426,8 +442,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -447,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -467,23 +486,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -491,7 +534,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -499,7 +542,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -507,7 +550,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -515,7 +558,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -523,7 +566,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -531,7 +574,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>

</xml_diff>

<commit_message>
add non decreasing numbers with n digits
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>medium</t>
+  </si>
+  <si>
+    <t>Mobile Numeric Keypad Problem</t>
+  </si>
+  <si>
+    <t>Total number of non-decreasing numbers with n digits</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,20 +533,44 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
add DP from g4g
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>number of binary strings without consecutive 1’s</t>
+  </si>
+  <si>
+    <t>Shortest Common Supersequence</t>
+  </si>
+  <si>
+    <t>Maximum number of A’s using given four keys</t>
+  </si>
+  <si>
+    <t>think about the transform func</t>
   </si>
 </sst>
 </file>
@@ -101,12 +110,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -121,9 +136,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -430,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +461,7 @@
     <col min="3" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,12 +686,47 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add one DP g4g
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>think about the transform func</t>
+  </si>
+  <si>
+    <t>Vertex_Cover_Problem</t>
+  </si>
+  <si>
+    <t>Weighted Job Scheduling</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +734,46 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add leetcode 114 flattern binary tree
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>leetcode 333</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
+  </si>
+  <si>
+    <t>leetcode 114</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,6 +852,23 @@
         <v>35</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Leetcode 222 Complete Tree Node
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>leetcode 114</t>
+  </si>
+  <si>
+    <t>Count Complete Tree Node</t>
+  </si>
+  <si>
+    <t>leetcode 222</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +875,23 @@
         <v>37</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Closest Binary Search Tree Value II
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="45">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>leetcode 222</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Preorder and Inorder Traversal</t>
+  </si>
+  <si>
+    <t>leetcode 105</t>
+  </si>
+  <si>
+    <t>Closest Binary Search Tree Value II</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>leetcode 272</t>
   </si>
 </sst>
 </file>
@@ -490,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,6 +907,40 @@
         <v>39</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Binary Tree Upside Down
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>leetcode 272</t>
+  </si>
+  <si>
+    <t>Binary Tree Upside Down</t>
+  </si>
+  <si>
+    <t>leetcode 156</t>
   </si>
 </sst>
 </file>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,6 +947,23 @@
         <v>44</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Binary Tree Postorder Traversal
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>leetcode 156</t>
+  </si>
+  <si>
+    <t>Binary Tree Postorder Traversal</t>
+  </si>
+  <si>
+    <t>leetcode 145</t>
   </si>
 </sst>
 </file>
@@ -511,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,6 +970,23 @@
         <v>46</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Binary Tree Maximum Path Sum
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>leetcode 145</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>leetcode 124</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,6 +993,23 @@
         <v>48</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bottom View of a Binary Tree
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>leetcode 124</t>
+  </si>
+  <si>
+    <t>Bottom View of a Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
@@ -1010,6 +1013,23 @@
         <v>50</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove nodes on root to leaf paths of length
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Bottom View of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Print Nodes in Top View of Binary Tree</t>
+  </si>
+  <si>
+    <t>Remove nodes on root to leaf paths of length &lt; K</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,6 +1036,40 @@
         <v>5</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Graph BFS and DFS
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="57">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>Remove nodes on root to leaf paths of length &lt; K</t>
+  </si>
+  <si>
+    <t>Directed Graph</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>BFS, DFS</t>
   </si>
 </sst>
 </file>
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,6 +1079,26 @@
         <v>5</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Snake and Ladder Problem
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="69">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>BFS</t>
+  </si>
+  <si>
+    <t>Snake and Ladder Problem</t>
   </si>
 </sst>
 </file>
@@ -574,23 +577,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -611,7 +614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -631,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -651,7 +654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -671,7 +674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -691,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -711,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -731,7 +734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -751,7 +754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -771,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -791,7 +794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -811,7 +814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -831,7 +834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -854,7 +857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -874,7 +877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -891,7 +894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -908,7 +911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -925,7 +928,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -942,7 +945,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -959,7 +962,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -976,7 +979,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -993,7 +996,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1061,13 +1064,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1078,13 +1082,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1095,13 +1100,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1112,14 +1118,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1132,14 +1138,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1152,14 +1158,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1175,14 +1181,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1195,14 +1201,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1213,6 +1219,26 @@
       </c>
       <c r="F33" s="1" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Number of Islands union find
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -221,6 +221,15 @@
   </si>
   <si>
     <t>Snake and Ladder Problem</t>
+  </si>
+  <si>
+    <t>Alien Dictionary</t>
+  </si>
+  <si>
+    <t>leetcode 269</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
   </si>
 </sst>
 </file>
@@ -577,23 +586,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -614,7 +623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -634,7 +643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -654,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -674,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -694,7 +703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -714,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -734,7 +743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -754,7 +763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -774,7 +783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -794,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -814,7 +823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -834,7 +843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -857,7 +866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -877,7 +886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -894,7 +903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -911,7 +920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -928,7 +937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -945,7 +954,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -962,7 +971,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -979,7 +988,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1047,7 +1056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1064,7 +1073,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1082,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1118,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1181,7 +1190,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1221,7 +1230,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1239,6 +1248,34 @@
       </c>
       <c r="F34" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Number of Islands II
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="76">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -230,6 +230,18 @@
   </si>
   <si>
     <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>Graph/UF</t>
+  </si>
+  <si>
+    <t>leetcode 200</t>
+  </si>
+  <si>
+    <t>Number of Islands II</t>
+  </si>
+  <si>
+    <t>leetcode 305</t>
   </si>
 </sst>
 </file>
@@ -586,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,6 +1289,32 @@
       <c r="B36" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="D36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
umber of Connected Components in an Undirected Graph
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="78">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>leetcode 305</t>
+  </si>
+  <si>
+    <t>Number of Connected Components in an Undirected Graph</t>
+  </si>
+  <si>
+    <t>leetcode 323</t>
   </si>
 </sst>
 </file>
@@ -598,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,6 +1322,23 @@
         <v>75</v>
       </c>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
back tracking + Memorize
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="111">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -341,6 +341,12 @@
   </si>
   <si>
     <t>use both backtracing and recursion</t>
+  </si>
+  <si>
+    <t>Longest Increasing Path in a Matrix</t>
+  </si>
+  <si>
+    <t>leetcode 329</t>
   </si>
 </sst>
 </file>
@@ -698,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,6 +1718,26 @@
         <v>108</v>
       </c>
     </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Segment Tree, Binary Index Tree
</commit_message>
<xml_diff>
--- a/Question_List.xlsx
+++ b/Question_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="122">
   <si>
     <t>Largest Independent Set Problem</t>
   </si>
@@ -371,6 +371,15 @@
   </si>
   <si>
     <t>lintcode 205</t>
+  </si>
+  <si>
+    <t>Range Sum Query - Mutable</t>
+  </si>
+  <si>
+    <t>lintcode 307</t>
+  </si>
+  <si>
+    <t>SegmentTree/BIT</t>
   </si>
 </sst>
 </file>
@@ -728,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +749,7 @@
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.28515625" customWidth="1"/>
@@ -1982,6 +1991,26 @@
         <v>118</v>
       </c>
     </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="3">
+        <v>5</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>